<commit_message>
changed file path method for compatability with other OS's
</commit_message>
<xml_diff>
--- a/data/rivers.xlsx
+++ b/data/rivers.xlsx
@@ -1075,9 +1075,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://www.chimuadventures.com/blog/wp-content/uploads/2016/07/The-Amazon-River-as-it-snakes-its-way-through-the-Amazon-Rainforest.jpg</t>
-  </si>
-  <si>
     <t>https://afrotourism.com/wp-content/uploads/2014/11/bluenileriver2.jpg</t>
   </si>
   <si>
@@ -1142,6 +1139,9 @@
   </si>
   <si>
     <t>https://media.istockphoto.com/photos/the-uglich-kremlin-aerial-view-picture-id695048582?k=6&amp;m=695048582&amp;s=612x612&amp;w=0&amp;h=zEVh5cVEaCzfX94xOTd0ulXd6iTqCVhOwhtgtWU-d-4=</t>
+  </si>
+  <si>
+    <t>https://www.rainforest-alliance.org/sites/default/files/2016-09/amazon-rainforest.jpg</t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1317,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1329,20 +1329,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1630,7 +1630,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,7 +1676,7 @@
         <v>88</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP($A2,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1708,7 +1708,7 @@
         <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP($A3,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP($A4,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1772,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C5" t="str">
         <f>VLOOKUP($A5,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1804,7 +1804,7 @@
         <v>297</v>
       </c>
       <c r="B6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C6" t="str">
         <f>VLOOKUP($A6,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1836,7 +1836,7 @@
         <v>207</v>
       </c>
       <c r="B7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP($A7,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1868,7 +1868,7 @@
         <v>276</v>
       </c>
       <c r="B8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C8" t="str">
         <f>VLOOKUP($A8,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1900,7 +1900,7 @@
         <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP($A9,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1932,7 +1932,7 @@
         <v>298</v>
       </c>
       <c r="B10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C10" t="str">
         <f>VLOOKUP($A10,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1964,7 +1964,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C11" t="str">
         <f>VLOOKUP($A11,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -1996,7 +1996,7 @@
         <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C12" t="str">
         <f>VLOOKUP($A12,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2028,7 +2028,7 @@
         <v>299</v>
       </c>
       <c r="B13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C13" t="str">
         <f>VLOOKUP($A13,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2060,7 +2060,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C14" t="str">
         <f>VLOOKUP($A14,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2092,7 +2092,7 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C15" t="str">
         <f>VLOOKUP($A15,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2124,7 +2124,7 @@
         <v>300</v>
       </c>
       <c r="B16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C16" t="str">
         <f>VLOOKUP($A16,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2156,7 +2156,7 @@
         <v>138</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C17" t="str">
         <f>VLOOKUP($A17,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2188,7 +2188,7 @@
         <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C18" t="str">
         <f>VLOOKUP($A18,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2220,7 +2220,7 @@
         <v>301</v>
       </c>
       <c r="B19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C19" t="str">
         <f>VLOOKUP($A19,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2252,7 +2252,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C20" t="str">
         <f>VLOOKUP($A20,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2284,7 +2284,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C21" t="str">
         <f>VLOOKUP($A21,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2316,7 +2316,7 @@
         <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C22" t="str">
         <f>VLOOKUP($A22,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2348,7 +2348,7 @@
         <v>144</v>
       </c>
       <c r="B23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C23" t="str">
         <f>VLOOKUP($A23,Format!$A:$J,MATCH(C$1,Format!$A$1:$J$1,0),0)</f>
@@ -2377,8 +2377,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B17" r:id="rId2"/>
+    <hyperlink ref="B17" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2408,13 +2407,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="27" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="30" t="s">
@@ -2423,41 +2422,41 @@
       <c r="F1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="27" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
+      <c r="A4" s="23">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3">
@@ -2475,13 +2474,13 @@
       <c r="G4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="4">
         <v>-6400</v>
       </c>
@@ -2491,13 +2490,13 @@
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="26"/>
-      <c r="H5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:9" ht="225" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>2</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3">
@@ -2515,13 +2514,13 @@
       <c r="G6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
-      <c r="B7" s="23"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="4">
         <v>-6650</v>
       </c>
@@ -2531,10 +2530,10 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="26"/>
-      <c r="H7" s="23"/>
+      <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24">
+      <c r="A8" s="29">
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2555,12 +2554,12 @@
       <c r="G8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
@@ -2573,7 +2572,7 @@
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
       <c r="G9" s="26"/>
-      <c r="H9" s="23"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -2628,7 +2627,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
+      <c r="A12" s="29">
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2649,12 +2648,12 @@
       <c r="G12" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
@@ -2663,7 +2662,7 @@
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
       <c r="G13" s="26"/>
-      <c r="H13" s="23"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
@@ -2736,10 +2735,10 @@
       <c r="F16" s="25">
         <v>41800</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="24" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2752,11 +2751,11 @@
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="24">
+      <c r="A18" s="29">
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2777,12 +2776,12 @@
       <c r="G18" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="8" t="s">
         <v>31</v>
       </c>
@@ -2791,7 +2790,7 @@
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
-      <c r="H19" s="23"/>
+      <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
@@ -2820,7 +2819,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24">
+      <c r="A21" s="29">
         <v>12</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -2841,12 +2840,12 @@
       <c r="G21" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="24" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="8" t="s">
         <v>57</v>
       </c>
@@ -2855,7 +2854,7 @@
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
       <c r="G22" s="26"/>
-      <c r="H22" s="23"/>
+      <c r="H22" s="24"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
@@ -3144,7 +3143,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="29">
+      <c r="A34" s="23">
         <v>24</v>
       </c>
       <c r="B34" s="26" t="s">
@@ -3162,15 +3161,15 @@
       <c r="F34" s="25">
         <v>3300</v>
       </c>
-      <c r="G34" s="23" t="s">
+      <c r="G34" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H34" s="23" t="s">
+      <c r="H34" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="26"/>
       <c r="C35" s="3">
         <v>-2900</v>
@@ -3180,8 +3179,8 @@
       </c>
       <c r="E35" s="25"/>
       <c r="F35" s="25"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
@@ -3210,7 +3209,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="24">
+      <c r="A37" s="29">
         <v>26</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -3231,12 +3230,12 @@
       <c r="G37" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="H37" s="23" t="s">
+      <c r="H37" s="24" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="8" t="s">
         <v>132</v>
       </c>
@@ -3245,7 +3244,7 @@
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
-      <c r="H38" s="23"/>
+      <c r="H38" s="24"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
@@ -3361,7 +3360,7 @@
       <c r="C43" s="25">
         <v>2693</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="24" t="s">
         <v>146</v>
       </c>
       <c r="E43" s="25">
@@ -3373,7 +3372,7 @@
       <c r="G43" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="H43" s="23" t="s">
+      <c r="H43" s="24" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3382,12 +3381,12 @@
       <c r="B44" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="23"/>
+      <c r="H44" s="24"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
@@ -3722,7 +3721,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="27">
+      <c r="A58" s="31">
         <v>45</v>
       </c>
       <c r="B58" s="26" t="s">
@@ -3743,12 +3742,12 @@
       <c r="G58" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H58" s="23" t="s">
+      <c r="H58" s="24" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
+      <c r="A59" s="31"/>
       <c r="B59" s="26"/>
       <c r="C59" s="25"/>
       <c r="D59" s="25"/>
@@ -3757,7 +3756,7 @@
       </c>
       <c r="F59" s="25"/>
       <c r="G59" s="26"/>
-      <c r="H59" s="23"/>
+      <c r="H59" s="24"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
@@ -3994,7 +3993,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="24">
+      <c r="A69" s="29">
         <v>55</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -4015,12 +4014,12 @@
       <c r="G69" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="H69" s="23" t="s">
+      <c r="H69" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
+      <c r="A70" s="29"/>
       <c r="B70" s="8" t="s">
         <v>104</v>
       </c>
@@ -4029,7 +4028,7 @@
       <c r="E70" s="25"/>
       <c r="F70" s="25"/>
       <c r="G70" s="26"/>
-      <c r="H70" s="23"/>
+      <c r="H70" s="24"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
@@ -5615,46 +5614,39 @@
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
     <mergeCell ref="H34:H35"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
@@ -5669,39 +5661,46 @@
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" tooltip="Atlantic Ocean" display="https://en.wikipedia.org/wiki/Atlantic_Ocean"/>
@@ -6511,7 +6510,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B18" t="s">
         <v>308</v>

</xml_diff>